<commit_message>
Fill in most topics
</commit_message>
<xml_diff>
--- a/data-viz/inputs/report_outline_1.xlsx
+++ b/data-viz/inputs/report_outline_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/EU Subnational/EU-S Data/reports/eu-gpp-report/data-viz/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhabiby\Documents\GitHub\eu-gpp-report\data-viz\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_B99231273C69EBC4C805B6D83FDC14E2921C2AF0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C88FEE-AF35-45A1-8870-9E28D9C9683A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1746E86-9C4F-44D5-A1B1-2FACC9C2F412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outline" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="766">
   <si>
     <t>chapter</t>
   </si>
@@ -2276,6 +2276,54 @@
   </si>
   <si>
     <t>Civic Participation B</t>
+  </si>
+  <si>
+    <t>Corruption Perceptions</t>
+  </si>
+  <si>
+    <t>Justice System Evaluation</t>
+  </si>
+  <si>
+    <t>Problem Resolution</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Security Violence</t>
+  </si>
+  <si>
+    <t>Law Enforcement Performance</t>
+  </si>
+  <si>
+    <t>Criminal Justice Performance</t>
+  </si>
+  <si>
+    <t>Perceptions on Authoritarian Behavior</t>
+  </si>
+  <si>
+    <t>Civic Participation A</t>
+  </si>
+  <si>
+    <t>Civic Participation A Civic Participation B</t>
+  </si>
+  <si>
+    <t>Corruption Change</t>
+  </si>
+  <si>
+    <t>Opinions regarding Corruption</t>
+  </si>
+  <si>
+    <t>Corruption</t>
+  </si>
+  <si>
+    <t>Bribe Victimization</t>
+  </si>
+  <si>
+    <t>Information Provision</t>
+  </si>
+  <si>
+    <t>Information Requests</t>
   </si>
 </sst>
 </file>
@@ -2611,19 +2659,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P86" sqref="P86"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H140" sqref="H140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="149.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="149.36328125" customWidth="1"/>
+    <col min="7" max="7" width="20.54296875" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2664,7 +2712,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2705,7 +2753,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2746,7 +2794,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2787,7 +2835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2828,7 +2876,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2850,6 +2898,9 @@
       <c r="G6" t="s">
         <v>41</v>
       </c>
+      <c r="H6" t="s">
+        <v>750</v>
+      </c>
       <c r="I6" t="s">
         <v>42</v>
       </c>
@@ -2866,7 +2917,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2888,6 +2939,9 @@
       <c r="G7" t="s">
         <v>48</v>
       </c>
+      <c r="H7" t="s">
+        <v>750</v>
+      </c>
       <c r="I7" t="s">
         <v>42</v>
       </c>
@@ -2904,7 +2958,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2926,6 +2980,9 @@
       <c r="G8" t="s">
         <v>52</v>
       </c>
+      <c r="H8" t="s">
+        <v>750</v>
+      </c>
       <c r="I8" t="s">
         <v>42</v>
       </c>
@@ -2942,7 +2999,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2964,6 +3021,9 @@
       <c r="G9" t="s">
         <v>56</v>
       </c>
+      <c r="H9" t="s">
+        <v>750</v>
+      </c>
       <c r="I9" t="s">
         <v>42</v>
       </c>
@@ -2980,7 +3040,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3002,6 +3062,9 @@
       <c r="G10" t="s">
         <v>63</v>
       </c>
+      <c r="H10" t="s">
+        <v>751</v>
+      </c>
       <c r="I10" t="s">
         <v>64</v>
       </c>
@@ -3018,7 +3081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3040,6 +3103,9 @@
       <c r="G11" t="s">
         <v>69</v>
       </c>
+      <c r="H11" t="s">
+        <v>751</v>
+      </c>
       <c r="I11" t="s">
         <v>64</v>
       </c>
@@ -3056,7 +3122,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3078,6 +3144,9 @@
       <c r="G12" t="s">
         <v>74</v>
       </c>
+      <c r="H12" t="s">
+        <v>751</v>
+      </c>
       <c r="I12" t="s">
         <v>64</v>
       </c>
@@ -3094,7 +3163,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3116,6 +3185,9 @@
       <c r="G13" t="s">
         <v>79</v>
       </c>
+      <c r="H13" t="s">
+        <v>751</v>
+      </c>
       <c r="I13" t="s">
         <v>64</v>
       </c>
@@ -3132,7 +3204,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3154,6 +3226,9 @@
       <c r="G14" t="s">
         <v>84</v>
       </c>
+      <c r="H14" t="s">
+        <v>751</v>
+      </c>
       <c r="I14" t="s">
         <v>64</v>
       </c>
@@ -3170,7 +3245,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3192,6 +3267,9 @@
       <c r="G15" t="s">
         <v>89</v>
       </c>
+      <c r="H15" t="s">
+        <v>751</v>
+      </c>
       <c r="I15" t="s">
         <v>64</v>
       </c>
@@ -3208,7 +3286,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3230,6 +3308,9 @@
       <c r="G16" t="s">
         <v>94</v>
       </c>
+      <c r="H16" t="s">
+        <v>751</v>
+      </c>
       <c r="I16" t="s">
         <v>64</v>
       </c>
@@ -3246,7 +3327,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3268,6 +3349,9 @@
       <c r="G17" t="s">
         <v>99</v>
       </c>
+      <c r="H17" t="s">
+        <v>751</v>
+      </c>
       <c r="I17" t="s">
         <v>64</v>
       </c>
@@ -3284,7 +3368,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3306,6 +3390,9 @@
       <c r="G18" t="s">
         <v>104</v>
       </c>
+      <c r="H18" t="s">
+        <v>751</v>
+      </c>
       <c r="I18" t="s">
         <v>64</v>
       </c>
@@ -3322,7 +3409,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3357,7 +3444,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3392,7 +3479,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3427,7 +3514,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3462,7 +3549,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -3497,7 +3584,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3532,7 +3619,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -3567,7 +3654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -3602,7 +3689,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3637,7 +3724,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -3659,6 +3746,9 @@
       <c r="G28" t="s">
         <v>155</v>
       </c>
+      <c r="H28" t="s">
+        <v>752</v>
+      </c>
       <c r="I28" t="s">
         <v>156</v>
       </c>
@@ -3675,7 +3765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -3710,7 +3800,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3745,7 +3835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -3767,6 +3857,9 @@
       <c r="G31" t="s">
         <v>172</v>
       </c>
+      <c r="H31" t="s">
+        <v>753</v>
+      </c>
       <c r="I31" t="s">
         <v>173</v>
       </c>
@@ -3783,7 +3876,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -3805,6 +3898,9 @@
       <c r="G32" t="s">
         <v>178</v>
       </c>
+      <c r="H32" t="s">
+        <v>753</v>
+      </c>
       <c r="I32" t="s">
         <v>173</v>
       </c>
@@ -3821,7 +3917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -3843,6 +3939,9 @@
       <c r="G33" t="s">
         <v>184</v>
       </c>
+      <c r="H33" t="s">
+        <v>754</v>
+      </c>
       <c r="I33" t="s">
         <v>161</v>
       </c>
@@ -3859,7 +3958,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -3881,6 +3980,9 @@
       <c r="G34" t="s">
         <v>189</v>
       </c>
+      <c r="H34" t="s">
+        <v>754</v>
+      </c>
       <c r="I34" t="s">
         <v>161</v>
       </c>
@@ -3897,7 +3999,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -3919,6 +4021,9 @@
       <c r="G35" t="s">
         <v>194</v>
       </c>
+      <c r="H35" t="s">
+        <v>754</v>
+      </c>
       <c r="I35" t="s">
         <v>161</v>
       </c>
@@ -3935,7 +4040,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -3957,6 +4062,9 @@
       <c r="G36" t="s">
         <v>199</v>
       </c>
+      <c r="H36" t="s">
+        <v>754</v>
+      </c>
       <c r="I36" t="s">
         <v>161</v>
       </c>
@@ -3973,7 +4081,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -3995,6 +4103,9 @@
       <c r="G37" t="s">
         <v>204</v>
       </c>
+      <c r="H37" t="s">
+        <v>754</v>
+      </c>
       <c r="I37" t="s">
         <v>161</v>
       </c>
@@ -4011,7 +4122,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -4033,6 +4144,9 @@
       <c r="G38" t="s">
         <v>209</v>
       </c>
+      <c r="H38" t="s">
+        <v>754</v>
+      </c>
       <c r="I38" t="s">
         <v>161</v>
       </c>
@@ -4049,7 +4163,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -4071,6 +4185,9 @@
       <c r="G39" t="s">
         <v>214</v>
       </c>
+      <c r="H39" t="s">
+        <v>754</v>
+      </c>
       <c r="I39" t="s">
         <v>161</v>
       </c>
@@ -4087,7 +4204,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -4109,6 +4226,9 @@
       <c r="G40" t="s">
         <v>220</v>
       </c>
+      <c r="H40" t="s">
+        <v>755</v>
+      </c>
       <c r="I40" t="s">
         <v>64</v>
       </c>
@@ -4125,7 +4245,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -4147,6 +4267,9 @@
       <c r="G41" t="s">
         <v>225</v>
       </c>
+      <c r="H41" t="s">
+        <v>755</v>
+      </c>
       <c r="I41" t="s">
         <v>64</v>
       </c>
@@ -4163,7 +4286,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -4185,6 +4308,9 @@
       <c r="G42" t="s">
         <v>230</v>
       </c>
+      <c r="H42" t="s">
+        <v>755</v>
+      </c>
       <c r="I42" t="s">
         <v>64</v>
       </c>
@@ -4201,7 +4327,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -4223,6 +4349,9 @@
       <c r="G43" t="s">
         <v>235</v>
       </c>
+      <c r="H43" t="s">
+        <v>755</v>
+      </c>
       <c r="I43" t="s">
         <v>64</v>
       </c>
@@ -4239,7 +4368,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -4261,6 +4390,9 @@
       <c r="G44" t="s">
         <v>240</v>
       </c>
+      <c r="H44" t="s">
+        <v>755</v>
+      </c>
       <c r="I44" t="s">
         <v>64</v>
       </c>
@@ -4277,7 +4409,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -4299,6 +4431,9 @@
       <c r="G45" t="s">
         <v>245</v>
       </c>
+      <c r="H45" t="s">
+        <v>755</v>
+      </c>
       <c r="I45" t="s">
         <v>64</v>
       </c>
@@ -4315,7 +4450,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -4337,6 +4472,9 @@
       <c r="G46" t="s">
         <v>250</v>
       </c>
+      <c r="H46" t="s">
+        <v>755</v>
+      </c>
       <c r="I46" t="s">
         <v>64</v>
       </c>
@@ -4353,7 +4491,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -4375,6 +4513,9 @@
       <c r="G47" t="s">
         <v>254</v>
       </c>
+      <c r="H47" t="s">
+        <v>755</v>
+      </c>
       <c r="I47" t="s">
         <v>64</v>
       </c>
@@ -4391,7 +4532,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -4413,6 +4554,9 @@
       <c r="G48" t="s">
         <v>259</v>
       </c>
+      <c r="H48" t="s">
+        <v>756</v>
+      </c>
       <c r="I48" t="s">
         <v>64</v>
       </c>
@@ -4429,7 +4573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -4451,6 +4595,9 @@
       <c r="G49" t="s">
         <v>264</v>
       </c>
+      <c r="H49" t="s">
+        <v>756</v>
+      </c>
       <c r="I49" t="s">
         <v>64</v>
       </c>
@@ -4467,7 +4614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -4489,6 +4636,9 @@
       <c r="G50" t="s">
         <v>270</v>
       </c>
+      <c r="H50" t="s">
+        <v>756</v>
+      </c>
       <c r="I50" t="s">
         <v>64</v>
       </c>
@@ -4505,7 +4655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -4527,6 +4677,9 @@
       <c r="G51" t="s">
         <v>275</v>
       </c>
+      <c r="H51" t="s">
+        <v>756</v>
+      </c>
       <c r="I51" t="s">
         <v>64</v>
       </c>
@@ -4543,7 +4696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -4565,6 +4718,9 @@
       <c r="G52" t="s">
         <v>280</v>
       </c>
+      <c r="H52" t="s">
+        <v>756</v>
+      </c>
       <c r="I52" t="s">
         <v>64</v>
       </c>
@@ -4581,7 +4737,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -4603,6 +4759,9 @@
       <c r="G53" t="s">
         <v>286</v>
       </c>
+      <c r="H53" t="s">
+        <v>755</v>
+      </c>
       <c r="I53" t="s">
         <v>64</v>
       </c>
@@ -4619,7 +4778,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -4641,6 +4800,9 @@
       <c r="G54" t="s">
         <v>291</v>
       </c>
+      <c r="H54" t="s">
+        <v>755</v>
+      </c>
       <c r="I54" t="s">
         <v>64</v>
       </c>
@@ -4657,7 +4819,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -4679,6 +4841,9 @@
       <c r="G55" t="s">
         <v>296</v>
       </c>
+      <c r="H55" t="s">
+        <v>755</v>
+      </c>
       <c r="I55" t="s">
         <v>64</v>
       </c>
@@ -4695,7 +4860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -4717,6 +4882,9 @@
       <c r="G56" t="s">
         <v>301</v>
       </c>
+      <c r="H56" t="s">
+        <v>756</v>
+      </c>
       <c r="I56" t="s">
         <v>64</v>
       </c>
@@ -4733,7 +4901,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -4755,6 +4923,9 @@
       <c r="G57" t="s">
         <v>306</v>
       </c>
+      <c r="H57" t="s">
+        <v>756</v>
+      </c>
       <c r="I57" t="s">
         <v>64</v>
       </c>
@@ -4771,7 +4942,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -4793,6 +4964,9 @@
       <c r="G58" t="s">
         <v>311</v>
       </c>
+      <c r="H58" t="s">
+        <v>756</v>
+      </c>
       <c r="I58" t="s">
         <v>64</v>
       </c>
@@ -4809,7 +4983,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -4831,6 +5005,9 @@
       <c r="G59" t="s">
         <v>316</v>
       </c>
+      <c r="H59" t="s">
+        <v>756</v>
+      </c>
       <c r="I59" t="s">
         <v>64</v>
       </c>
@@ -4847,7 +5024,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>319</v>
       </c>
@@ -4869,6 +5046,9 @@
       <c r="G60" t="s">
         <v>324</v>
       </c>
+      <c r="H60" t="s">
+        <v>757</v>
+      </c>
       <c r="I60" t="s">
         <v>64</v>
       </c>
@@ -4885,7 +5065,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>319</v>
       </c>
@@ -4907,6 +5087,9 @@
       <c r="G61" t="s">
         <v>330</v>
       </c>
+      <c r="H61" t="s">
+        <v>757</v>
+      </c>
       <c r="I61" t="s">
         <v>64</v>
       </c>
@@ -4923,7 +5106,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>319</v>
       </c>
@@ -4945,6 +5128,9 @@
       <c r="G62" t="s">
         <v>335</v>
       </c>
+      <c r="H62" t="s">
+        <v>757</v>
+      </c>
       <c r="I62" t="s">
         <v>64</v>
       </c>
@@ -4961,7 +5147,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>319</v>
       </c>
@@ -4983,6 +5169,9 @@
       <c r="G63" t="s">
         <v>340</v>
       </c>
+      <c r="H63" t="s">
+        <v>757</v>
+      </c>
       <c r="I63" t="s">
         <v>64</v>
       </c>
@@ -4999,7 +5188,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>319</v>
       </c>
@@ -5021,6 +5210,9 @@
       <c r="G64" t="s">
         <v>345</v>
       </c>
+      <c r="H64" t="s">
+        <v>757</v>
+      </c>
       <c r="I64" t="s">
         <v>64</v>
       </c>
@@ -5037,7 +5229,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>319</v>
       </c>
@@ -5059,6 +5251,9 @@
       <c r="G65" t="s">
         <v>350</v>
       </c>
+      <c r="H65" t="s">
+        <v>757</v>
+      </c>
       <c r="I65" t="s">
         <v>64</v>
       </c>
@@ -5075,7 +5270,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>319</v>
       </c>
@@ -5097,6 +5292,9 @@
       <c r="G66" t="s">
         <v>355</v>
       </c>
+      <c r="H66" t="s">
+        <v>757</v>
+      </c>
       <c r="I66" t="s">
         <v>64</v>
       </c>
@@ -5113,7 +5311,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>319</v>
       </c>
@@ -5135,6 +5333,9 @@
       <c r="G67" t="s">
         <v>360</v>
       </c>
+      <c r="H67" t="s">
+        <v>757</v>
+      </c>
       <c r="I67" t="s">
         <v>64</v>
       </c>
@@ -5151,7 +5352,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>319</v>
       </c>
@@ -5173,6 +5374,9 @@
       <c r="G68" t="s">
         <v>365</v>
       </c>
+      <c r="H68" t="s">
+        <v>757</v>
+      </c>
       <c r="I68" t="s">
         <v>64</v>
       </c>
@@ -5189,7 +5393,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>319</v>
       </c>
@@ -5211,6 +5415,9 @@
       <c r="G69" t="s">
         <v>371</v>
       </c>
+      <c r="H69" t="s">
+        <v>757</v>
+      </c>
       <c r="I69" t="s">
         <v>64</v>
       </c>
@@ -5227,7 +5434,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>319</v>
       </c>
@@ -5249,6 +5456,9 @@
       <c r="G70" t="s">
         <v>376</v>
       </c>
+      <c r="H70" t="s">
+        <v>757</v>
+      </c>
       <c r="I70" t="s">
         <v>64</v>
       </c>
@@ -5265,7 +5475,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>319</v>
       </c>
@@ -5287,6 +5497,9 @@
       <c r="G71" t="s">
         <v>381</v>
       </c>
+      <c r="H71" t="s">
+        <v>757</v>
+      </c>
       <c r="I71" t="s">
         <v>64</v>
       </c>
@@ -5303,7 +5516,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>319</v>
       </c>
@@ -5325,6 +5538,9 @@
       <c r="G72" t="s">
         <v>386</v>
       </c>
+      <c r="H72" t="s">
+        <v>757</v>
+      </c>
       <c r="I72" t="s">
         <v>64</v>
       </c>
@@ -5341,7 +5557,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>319</v>
       </c>
@@ -5363,6 +5579,9 @@
       <c r="G73" t="s">
         <v>391</v>
       </c>
+      <c r="H73" t="s">
+        <v>757</v>
+      </c>
       <c r="I73" t="s">
         <v>64</v>
       </c>
@@ -5379,7 +5598,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>319</v>
       </c>
@@ -5401,6 +5620,9 @@
       <c r="G74" t="s">
         <v>396</v>
       </c>
+      <c r="H74" t="s">
+        <v>757</v>
+      </c>
       <c r="I74" t="s">
         <v>64</v>
       </c>
@@ -5417,7 +5639,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>319</v>
       </c>
@@ -5439,6 +5661,9 @@
       <c r="G75" t="s">
         <v>402</v>
       </c>
+      <c r="H75" t="s">
+        <v>751</v>
+      </c>
       <c r="I75" t="s">
         <v>64</v>
       </c>
@@ -5455,7 +5680,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>319</v>
       </c>
@@ -5477,6 +5702,9 @@
       <c r="G76" t="s">
         <v>407</v>
       </c>
+      <c r="H76" t="s">
+        <v>751</v>
+      </c>
       <c r="I76" t="s">
         <v>64</v>
       </c>
@@ -5493,7 +5721,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>319</v>
       </c>
@@ -5515,6 +5743,9 @@
       <c r="G77" t="s">
         <v>412</v>
       </c>
+      <c r="H77" t="s">
+        <v>757</v>
+      </c>
       <c r="I77" t="s">
         <v>64</v>
       </c>
@@ -5531,7 +5762,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>319</v>
       </c>
@@ -5553,6 +5784,9 @@
       <c r="G78" t="s">
         <v>417</v>
       </c>
+      <c r="H78" t="s">
+        <v>757</v>
+      </c>
       <c r="I78" t="s">
         <v>64</v>
       </c>
@@ -5569,7 +5803,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>319</v>
       </c>
@@ -5591,6 +5825,9 @@
       <c r="G79" t="s">
         <v>422</v>
       </c>
+      <c r="H79" t="s">
+        <v>757</v>
+      </c>
       <c r="I79" t="s">
         <v>64</v>
       </c>
@@ -5607,7 +5844,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>319</v>
       </c>
@@ -5629,6 +5866,9 @@
       <c r="G80" t="s">
         <v>429</v>
       </c>
+      <c r="H80" t="s">
+        <v>758</v>
+      </c>
       <c r="I80" t="s">
         <v>64</v>
       </c>
@@ -5645,7 +5885,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>319</v>
       </c>
@@ -5667,6 +5907,9 @@
       <c r="G81" t="s">
         <v>434</v>
       </c>
+      <c r="H81" t="s">
+        <v>758</v>
+      </c>
       <c r="I81" t="s">
         <v>64</v>
       </c>
@@ -5683,7 +5926,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>319</v>
       </c>
@@ -5705,6 +5948,9 @@
       <c r="G82" t="s">
         <v>439</v>
       </c>
+      <c r="H82" t="s">
+        <v>749</v>
+      </c>
       <c r="I82" t="s">
         <v>64</v>
       </c>
@@ -5721,7 +5967,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>319</v>
       </c>
@@ -5743,6 +5989,9 @@
       <c r="G83" t="s">
         <v>444</v>
       </c>
+      <c r="H83" t="s">
+        <v>749</v>
+      </c>
       <c r="I83" t="s">
         <v>64</v>
       </c>
@@ -5759,7 +6008,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>319</v>
       </c>
@@ -5781,6 +6030,9 @@
       <c r="G84" t="s">
         <v>449</v>
       </c>
+      <c r="H84" t="s">
+        <v>749</v>
+      </c>
       <c r="I84" t="s">
         <v>64</v>
       </c>
@@ -5797,7 +6049,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>319</v>
       </c>
@@ -5819,6 +6071,9 @@
       <c r="G85" t="s">
         <v>454</v>
       </c>
+      <c r="H85" t="s">
+        <v>749</v>
+      </c>
       <c r="I85" t="s">
         <v>64</v>
       </c>
@@ -5835,7 +6090,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>319</v>
       </c>
@@ -5857,6 +6112,9 @@
       <c r="G86" t="s">
         <v>460</v>
       </c>
+      <c r="H86" t="s">
+        <v>758</v>
+      </c>
       <c r="I86" t="s">
         <v>64</v>
       </c>
@@ -5873,7 +6131,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>319</v>
       </c>
@@ -5895,6 +6153,9 @@
       <c r="G87" t="s">
         <v>465</v>
       </c>
+      <c r="H87" t="s">
+        <v>758</v>
+      </c>
       <c r="I87" t="s">
         <v>64</v>
       </c>
@@ -5911,7 +6172,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>319</v>
       </c>
@@ -5933,6 +6194,9 @@
       <c r="G88" t="s">
         <v>470</v>
       </c>
+      <c r="H88" t="s">
+        <v>758</v>
+      </c>
       <c r="I88" t="s">
         <v>64</v>
       </c>
@@ -5949,7 +6213,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>319</v>
       </c>
@@ -5990,7 +6254,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>319</v>
       </c>
@@ -6031,7 +6295,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>319</v>
       </c>
@@ -6072,7 +6336,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>319</v>
       </c>
@@ -6113,7 +6377,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>319</v>
       </c>
@@ -6135,6 +6399,9 @@
       <c r="G93" t="s">
         <v>496</v>
       </c>
+      <c r="H93" t="s">
+        <v>758</v>
+      </c>
       <c r="I93" t="s">
         <v>64</v>
       </c>
@@ -6151,7 +6418,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>319</v>
       </c>
@@ -6173,6 +6440,9 @@
       <c r="G94" t="s">
         <v>501</v>
       </c>
+      <c r="H94" t="s">
+        <v>758</v>
+      </c>
       <c r="I94" t="s">
         <v>64</v>
       </c>
@@ -6189,7 +6459,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>319</v>
       </c>
@@ -6211,6 +6481,9 @@
       <c r="G95" t="s">
         <v>507</v>
       </c>
+      <c r="H95" t="s">
+        <v>759</v>
+      </c>
       <c r="I95" t="s">
         <v>161</v>
       </c>
@@ -6227,7 +6500,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>319</v>
       </c>
@@ -6249,6 +6522,9 @@
       <c r="G96" t="s">
         <v>512</v>
       </c>
+      <c r="H96" t="s">
+        <v>759</v>
+      </c>
       <c r="I96" t="s">
         <v>161</v>
       </c>
@@ -6265,7 +6541,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>319</v>
       </c>
@@ -6287,6 +6563,9 @@
       <c r="G97" t="s">
         <v>517</v>
       </c>
+      <c r="H97" t="s">
+        <v>759</v>
+      </c>
       <c r="I97" t="s">
         <v>161</v>
       </c>
@@ -6303,7 +6582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>319</v>
       </c>
@@ -6325,6 +6604,9 @@
       <c r="G98" t="s">
         <v>522</v>
       </c>
+      <c r="H98" t="s">
+        <v>758</v>
+      </c>
       <c r="I98" t="s">
         <v>64</v>
       </c>
@@ -6341,7 +6623,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>319</v>
       </c>
@@ -6363,6 +6645,9 @@
       <c r="G99" t="s">
         <v>527</v>
       </c>
+      <c r="H99" t="s">
+        <v>758</v>
+      </c>
       <c r="I99" t="s">
         <v>64</v>
       </c>
@@ -6379,7 +6664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>319</v>
       </c>
@@ -6401,6 +6686,9 @@
       <c r="G100" t="s">
         <v>532</v>
       </c>
+      <c r="H100" t="s">
+        <v>749</v>
+      </c>
       <c r="I100" t="s">
         <v>64</v>
       </c>
@@ -6417,7 +6705,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>319</v>
       </c>
@@ -6439,6 +6727,9 @@
       <c r="G101" t="s">
         <v>537</v>
       </c>
+      <c r="H101" t="s">
+        <v>749</v>
+      </c>
       <c r="I101" t="s">
         <v>64</v>
       </c>
@@ -6455,7 +6746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>319</v>
       </c>
@@ -6477,6 +6768,9 @@
       <c r="G102" t="s">
         <v>543</v>
       </c>
+      <c r="H102" t="s">
+        <v>540</v>
+      </c>
       <c r="I102" t="s">
         <v>161</v>
       </c>
@@ -6493,7 +6787,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>319</v>
       </c>
@@ -6515,6 +6809,9 @@
       <c r="G103" t="s">
         <v>548</v>
       </c>
+      <c r="H103" t="s">
+        <v>540</v>
+      </c>
       <c r="I103" t="s">
         <v>161</v>
       </c>
@@ -6531,7 +6828,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>319</v>
       </c>
@@ -6553,6 +6850,9 @@
       <c r="G104" t="s">
         <v>553</v>
       </c>
+      <c r="H104" t="s">
+        <v>540</v>
+      </c>
       <c r="I104" t="s">
         <v>161</v>
       </c>
@@ -6569,7 +6869,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>319</v>
       </c>
@@ -6591,6 +6891,9 @@
       <c r="G105" t="s">
         <v>558</v>
       </c>
+      <c r="H105" t="s">
+        <v>540</v>
+      </c>
       <c r="I105" t="s">
         <v>161</v>
       </c>
@@ -6607,7 +6910,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>319</v>
       </c>
@@ -6629,6 +6932,9 @@
       <c r="G106" t="s">
         <v>563</v>
       </c>
+      <c r="H106" t="s">
+        <v>540</v>
+      </c>
       <c r="I106" t="s">
         <v>161</v>
       </c>
@@ -6645,7 +6951,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>319</v>
       </c>
@@ -6667,6 +6973,9 @@
       <c r="G107" t="s">
         <v>568</v>
       </c>
+      <c r="H107" t="s">
+        <v>540</v>
+      </c>
       <c r="I107" t="s">
         <v>161</v>
       </c>
@@ -6683,7 +6992,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>319</v>
       </c>
@@ -6705,6 +7014,9 @@
       <c r="G108" t="s">
         <v>573</v>
       </c>
+      <c r="H108" t="s">
+        <v>540</v>
+      </c>
       <c r="I108" t="s">
         <v>161</v>
       </c>
@@ -6721,7 +7033,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>319</v>
       </c>
@@ -6743,6 +7055,9 @@
       <c r="G109" t="s">
         <v>578</v>
       </c>
+      <c r="H109" t="s">
+        <v>540</v>
+      </c>
       <c r="I109" t="s">
         <v>161</v>
       </c>
@@ -6759,7 +7074,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>319</v>
       </c>
@@ -6781,6 +7096,9 @@
       <c r="G110" t="s">
         <v>583</v>
       </c>
+      <c r="H110" t="s">
+        <v>540</v>
+      </c>
       <c r="I110" t="s">
         <v>161</v>
       </c>
@@ -6797,7 +7115,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>319</v>
       </c>
@@ -6819,6 +7137,9 @@
       <c r="G111" t="s">
         <v>588</v>
       </c>
+      <c r="H111" t="s">
+        <v>540</v>
+      </c>
       <c r="I111" t="s">
         <v>161</v>
       </c>
@@ -6835,7 +7156,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>319</v>
       </c>
@@ -6857,6 +7178,9 @@
       <c r="G112" t="s">
         <v>593</v>
       </c>
+      <c r="H112" t="s">
+        <v>540</v>
+      </c>
       <c r="I112" t="s">
         <v>161</v>
       </c>
@@ -6873,7 +7197,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>319</v>
       </c>
@@ -6911,7 +7235,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>602</v>
       </c>
@@ -6933,6 +7257,9 @@
       <c r="G114" t="s">
         <v>607</v>
       </c>
+      <c r="H114" t="s">
+        <v>760</v>
+      </c>
       <c r="I114" t="s">
         <v>608</v>
       </c>
@@ -6949,7 +7276,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>602</v>
       </c>
@@ -6971,6 +7298,9 @@
       <c r="G115" t="s">
         <v>613</v>
       </c>
+      <c r="H115" t="s">
+        <v>761</v>
+      </c>
       <c r="I115" t="s">
         <v>64</v>
       </c>
@@ -6987,7 +7317,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>602</v>
       </c>
@@ -7009,6 +7339,9 @@
       <c r="G116" t="s">
         <v>618</v>
       </c>
+      <c r="H116" t="s">
+        <v>761</v>
+      </c>
       <c r="I116" t="s">
         <v>64</v>
       </c>
@@ -7025,7 +7358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>602</v>
       </c>
@@ -7047,6 +7380,9 @@
       <c r="G117" t="s">
         <v>623</v>
       </c>
+      <c r="H117" t="s">
+        <v>761</v>
+      </c>
       <c r="I117" t="s">
         <v>64</v>
       </c>
@@ -7063,7 +7399,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>602</v>
       </c>
@@ -7085,6 +7421,9 @@
       <c r="G118" t="s">
         <v>628</v>
       </c>
+      <c r="H118" t="s">
+        <v>761</v>
+      </c>
       <c r="I118" t="s">
         <v>64</v>
       </c>
@@ -7101,7 +7440,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>602</v>
       </c>
@@ -7123,6 +7462,9 @@
       <c r="G119" t="s">
         <v>633</v>
       </c>
+      <c r="H119" t="s">
+        <v>761</v>
+      </c>
       <c r="I119" t="s">
         <v>64</v>
       </c>
@@ -7139,7 +7481,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>602</v>
       </c>
@@ -7161,6 +7503,9 @@
       <c r="G120" t="s">
         <v>639</v>
       </c>
+      <c r="H120" t="s">
+        <v>762</v>
+      </c>
       <c r="I120" t="s">
         <v>42</v>
       </c>
@@ -7177,7 +7522,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>602</v>
       </c>
@@ -7199,6 +7544,9 @@
       <c r="G121" t="s">
         <v>644</v>
       </c>
+      <c r="H121" t="s">
+        <v>762</v>
+      </c>
       <c r="I121" t="s">
         <v>42</v>
       </c>
@@ -7215,7 +7563,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>602</v>
       </c>
@@ -7237,6 +7585,9 @@
       <c r="G122" t="s">
         <v>649</v>
       </c>
+      <c r="H122" t="s">
+        <v>762</v>
+      </c>
       <c r="I122" t="s">
         <v>42</v>
       </c>
@@ -7253,7 +7604,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>602</v>
       </c>
@@ -7275,6 +7626,9 @@
       <c r="G123" t="s">
         <v>41</v>
       </c>
+      <c r="H123" t="s">
+        <v>762</v>
+      </c>
       <c r="I123" t="s">
         <v>42</v>
       </c>
@@ -7291,7 +7645,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>602</v>
       </c>
@@ -7313,6 +7667,9 @@
       <c r="G124" t="s">
         <v>48</v>
       </c>
+      <c r="H124" t="s">
+        <v>762</v>
+      </c>
       <c r="I124" t="s">
         <v>42</v>
       </c>
@@ -7329,7 +7686,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>602</v>
       </c>
@@ -7351,6 +7708,9 @@
       <c r="G125" t="s">
         <v>52</v>
       </c>
+      <c r="H125" t="s">
+        <v>762</v>
+      </c>
       <c r="I125" t="s">
         <v>42</v>
       </c>
@@ -7367,7 +7727,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>602</v>
       </c>
@@ -7389,6 +7749,9 @@
       <c r="G126" t="s">
         <v>56</v>
       </c>
+      <c r="H126" t="s">
+        <v>762</v>
+      </c>
       <c r="I126" t="s">
         <v>42</v>
       </c>
@@ -7405,7 +7768,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>602</v>
       </c>
@@ -7427,6 +7790,9 @@
       <c r="G127" t="s">
         <v>660</v>
       </c>
+      <c r="H127" t="s">
+        <v>762</v>
+      </c>
       <c r="I127" t="s">
         <v>42</v>
       </c>
@@ -7443,7 +7809,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>602</v>
       </c>
@@ -7465,6 +7831,9 @@
       <c r="G128" t="s">
         <v>665</v>
       </c>
+      <c r="H128" t="s">
+        <v>762</v>
+      </c>
       <c r="I128" t="s">
         <v>42</v>
       </c>
@@ -7481,7 +7850,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>602</v>
       </c>
@@ -7503,6 +7872,9 @@
       <c r="G129" t="s">
         <v>670</v>
       </c>
+      <c r="H129" t="s">
+        <v>762</v>
+      </c>
       <c r="I129" t="s">
         <v>42</v>
       </c>
@@ -7519,7 +7891,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>602</v>
       </c>
@@ -7541,6 +7913,9 @@
       <c r="G130" t="s">
         <v>675</v>
       </c>
+      <c r="H130" t="s">
+        <v>762</v>
+      </c>
       <c r="I130" t="s">
         <v>42</v>
       </c>
@@ -7557,7 +7932,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>602</v>
       </c>
@@ -7579,6 +7954,9 @@
       <c r="G131" t="s">
         <v>681</v>
       </c>
+      <c r="H131" t="s">
+        <v>763</v>
+      </c>
       <c r="I131" t="s">
         <v>161</v>
       </c>
@@ -7595,7 +7973,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>602</v>
       </c>
@@ -7617,6 +7995,9 @@
       <c r="G132" t="s">
         <v>686</v>
       </c>
+      <c r="H132" t="s">
+        <v>763</v>
+      </c>
       <c r="I132" t="s">
         <v>161</v>
       </c>
@@ -7633,7 +8014,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>602</v>
       </c>
@@ -7655,6 +8036,9 @@
       <c r="G133" t="s">
         <v>691</v>
       </c>
+      <c r="H133" t="s">
+        <v>763</v>
+      </c>
       <c r="I133" t="s">
         <v>161</v>
       </c>
@@ -7671,7 +8055,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>602</v>
       </c>
@@ -7693,6 +8077,9 @@
       <c r="G134" t="s">
         <v>696</v>
       </c>
+      <c r="H134" t="s">
+        <v>763</v>
+      </c>
       <c r="I134" t="s">
         <v>161</v>
       </c>
@@ -7709,7 +8096,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>602</v>
       </c>
@@ -7731,6 +8118,9 @@
       <c r="G135" t="s">
         <v>701</v>
       </c>
+      <c r="H135" t="s">
+        <v>763</v>
+      </c>
       <c r="I135" t="s">
         <v>161</v>
       </c>
@@ -7747,7 +8137,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>602</v>
       </c>
@@ -7769,6 +8159,9 @@
       <c r="G136" t="s">
         <v>708</v>
       </c>
+      <c r="H136" t="s">
+        <v>764</v>
+      </c>
       <c r="I136" t="s">
         <v>64</v>
       </c>
@@ -7785,7 +8178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>602</v>
       </c>
@@ -7807,6 +8200,9 @@
       <c r="G137" t="s">
         <v>713</v>
       </c>
+      <c r="H137" t="s">
+        <v>764</v>
+      </c>
       <c r="I137" t="s">
         <v>64</v>
       </c>
@@ -7823,7 +8219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>602</v>
       </c>
@@ -7845,6 +8241,9 @@
       <c r="G138" t="s">
         <v>718</v>
       </c>
+      <c r="H138" t="s">
+        <v>764</v>
+      </c>
       <c r="I138" t="s">
         <v>64</v>
       </c>
@@ -7861,7 +8260,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>602</v>
       </c>
@@ -7883,6 +8282,9 @@
       <c r="G139" t="s">
         <v>723</v>
       </c>
+      <c r="H139" t="s">
+        <v>764</v>
+      </c>
       <c r="I139" t="s">
         <v>64</v>
       </c>
@@ -7899,7 +8301,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>602</v>
       </c>
@@ -7921,6 +8323,9 @@
       <c r="G140" t="s">
         <v>729</v>
       </c>
+      <c r="H140" t="s">
+        <v>765</v>
+      </c>
       <c r="I140" t="s">
         <v>730</v>
       </c>
@@ -7937,7 +8342,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>602</v>
       </c>
@@ -7959,6 +8364,9 @@
       <c r="G141" t="s">
         <v>735</v>
       </c>
+      <c r="H141" t="s">
+        <v>765</v>
+      </c>
       <c r="I141" t="s">
         <v>730</v>
       </c>
@@ -7975,7 +8383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>602</v>
       </c>
@@ -7997,6 +8405,9 @@
       <c r="G142" t="s">
         <v>740</v>
       </c>
+      <c r="H142" t="s">
+        <v>765</v>
+      </c>
       <c r="I142" t="s">
         <v>730</v>
       </c>
@@ -8013,7 +8424,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>602</v>
       </c>
@@ -8034,6 +8445,9 @@
       </c>
       <c r="G143" t="s">
         <v>745</v>
+      </c>
+      <c r="H143" t="s">
+        <v>765</v>
       </c>
       <c r="I143" t="s">
         <v>730</v>
@@ -8058,6 +8472,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="579d0760968303502ff8eb3a8a5e610f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6855c386bbcb23a4cad2dada315b1779" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -8306,15 +8729,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -8327,6 +8741,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E88BA6A-AC61-4AC2-A996-5A1D6BDE06E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B06C0B83-8F91-4FA8-B18E-5FF0700E1417}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8345,14 +8767,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E88BA6A-AC61-4AC2-A996-5A1D6BDE06E6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8432CF-B2BE-4FBE-BA17-BEF2C1145140}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
expand rows for chart 22
</commit_message>
<xml_diff>
--- a/data-viz/inputs/report_outline_1.xlsx
+++ b/data-viz/inputs/report_outline_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhabiby\Documents\GitHub\eu-gpp-report\data-viz\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1746E86-9C4F-44D5-A1B1-2FACC9C2F412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F4A626-9191-49EA-A01D-390A9F6068D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="771">
   <si>
     <t>chapter</t>
   </si>
@@ -2324,6 +2324,21 @@
   </si>
   <si>
     <t>Information Requests</t>
+  </si>
+  <si>
+    <t>q154</t>
+  </si>
+  <si>
+    <t>q155</t>
+  </si>
+  <si>
+    <t>Information and Advice</t>
+  </si>
+  <si>
+    <t>AJD_information</t>
+  </si>
+  <si>
+    <t>AJD_inst_advice</t>
   </si>
 </sst>
 </file>
@@ -2657,11 +2672,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M143"/>
+  <dimension ref="A1:M144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H140" sqref="H140"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3566,7 +3581,13 @@
         <v>129</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>766</v>
+      </c>
+      <c r="G23" t="s">
+        <v>769</v>
+      </c>
+      <c r="H23" t="s">
+        <v>768</v>
       </c>
       <c r="I23" t="s">
         <v>131</v>
@@ -3595,25 +3616,31 @@
         <v>107</v>
       </c>
       <c r="D24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F24" t="s">
-        <v>130</v>
+        <v>767</v>
+      </c>
+      <c r="G24" t="s">
+        <v>770</v>
+      </c>
+      <c r="H24" t="s">
+        <v>768</v>
       </c>
       <c r="I24" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J24" t="s">
         <v>20</v>
       </c>
       <c r="K24" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="L24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M24" t="s">
         <v>23</v>
@@ -3630,25 +3657,25 @@
         <v>107</v>
       </c>
       <c r="D25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F25" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="I25" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J25" t="s">
         <v>20</v>
       </c>
       <c r="K25" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="L25" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="M25" t="s">
         <v>23</v>
@@ -3665,25 +3692,25 @@
         <v>107</v>
       </c>
       <c r="D26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F26" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I26" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J26" t="s">
         <v>20</v>
       </c>
       <c r="K26" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="L26" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="M26" t="s">
         <v>23</v>
@@ -3700,25 +3727,25 @@
         <v>107</v>
       </c>
       <c r="D27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F27" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="I27" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J27" t="s">
         <v>20</v>
       </c>
       <c r="K27" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="L27" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="M27" t="s">
         <v>23</v>
@@ -3735,31 +3762,25 @@
         <v>107</v>
       </c>
       <c r="D28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F28" t="s">
-        <v>154</v>
-      </c>
-      <c r="G28" t="s">
-        <v>155</v>
-      </c>
-      <c r="H28" t="s">
-        <v>752</v>
+        <v>149</v>
       </c>
       <c r="I28" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="J28" t="s">
         <v>20</v>
       </c>
       <c r="K28" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L28" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="M28" t="s">
         <v>23</v>
@@ -3776,25 +3797,31 @@
         <v>107</v>
       </c>
       <c r="D29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E29" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F29" t="s">
-        <v>160</v>
+        <v>154</v>
+      </c>
+      <c r="G29" t="s">
+        <v>155</v>
+      </c>
+      <c r="H29" t="s">
+        <v>752</v>
       </c>
       <c r="I29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="J29" t="s">
         <v>20</v>
       </c>
       <c r="K29" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L29" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M29" t="s">
         <v>23</v>
@@ -3811,13 +3838,13 @@
         <v>107</v>
       </c>
       <c r="D30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F30" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I30" t="s">
         <v>161</v>
@@ -3826,10 +3853,10 @@
         <v>20</v>
       </c>
       <c r="K30" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="L30" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M30" t="s">
         <v>23</v>
@@ -3840,37 +3867,31 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>168</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>169</v>
+        <v>107</v>
       </c>
       <c r="D31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F31" t="s">
-        <v>171</v>
-      </c>
-      <c r="G31" t="s">
-        <v>172</v>
-      </c>
-      <c r="H31" t="s">
-        <v>753</v>
+        <v>165</v>
       </c>
       <c r="I31" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="J31" t="s">
         <v>20</v>
       </c>
       <c r="K31" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="L31" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="M31" t="s">
         <v>23</v>
@@ -3887,16 +3908,16 @@
         <v>169</v>
       </c>
       <c r="D32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F32" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="G32" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="H32" t="s">
         <v>753</v>
@@ -3908,10 +3929,10 @@
         <v>20</v>
       </c>
       <c r="K32" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="L32" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="M32" t="s">
         <v>23</v>
@@ -3925,37 +3946,37 @@
         <v>168</v>
       </c>
       <c r="C33" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="F33" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G33" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="H33" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="I33" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="J33" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="K33" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="L33" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="M33" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
@@ -3969,16 +3990,16 @@
         <v>181</v>
       </c>
       <c r="D34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E34" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F34" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="G34" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="H34" t="s">
         <v>754</v>
@@ -3990,10 +4011,10 @@
         <v>43</v>
       </c>
       <c r="K34" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="L34" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="M34" t="s">
         <v>46</v>
@@ -4010,16 +4031,16 @@
         <v>181</v>
       </c>
       <c r="D35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F35" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G35" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H35" t="s">
         <v>754</v>
@@ -4031,10 +4052,10 @@
         <v>43</v>
       </c>
       <c r="K35" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="L35" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="M35" t="s">
         <v>46</v>
@@ -4051,16 +4072,16 @@
         <v>181</v>
       </c>
       <c r="D36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F36" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G36" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H36" t="s">
         <v>754</v>
@@ -4072,10 +4093,10 @@
         <v>43</v>
       </c>
       <c r="K36" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="L36" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="M36" t="s">
         <v>46</v>
@@ -4092,16 +4113,16 @@
         <v>181</v>
       </c>
       <c r="D37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E37" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F37" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G37" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H37" t="s">
         <v>754</v>
@@ -4113,10 +4134,10 @@
         <v>43</v>
       </c>
       <c r="K37" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L37" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="M37" t="s">
         <v>46</v>
@@ -4133,16 +4154,16 @@
         <v>181</v>
       </c>
       <c r="D38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E38" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F38" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G38" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H38" t="s">
         <v>754</v>
@@ -4154,10 +4175,10 @@
         <v>43</v>
       </c>
       <c r="K38" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="L38" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="M38" t="s">
         <v>46</v>
@@ -4174,16 +4195,16 @@
         <v>181</v>
       </c>
       <c r="D39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E39" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F39" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="G39" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H39" t="s">
         <v>754</v>
@@ -4195,10 +4216,10 @@
         <v>43</v>
       </c>
       <c r="K39" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="L39" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="M39" t="s">
         <v>46</v>
@@ -4212,37 +4233,37 @@
         <v>168</v>
       </c>
       <c r="C40" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
       <c r="D40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E40" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F40" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G40" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="H40" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="I40" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="J40" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="K40" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="L40" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="M40" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
@@ -4256,16 +4277,16 @@
         <v>217</v>
       </c>
       <c r="D41">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E41" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F41" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G41" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H41" t="s">
         <v>755</v>
@@ -4277,10 +4298,10 @@
         <v>20</v>
       </c>
       <c r="K41" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="L41" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="M41" t="s">
         <v>23</v>
@@ -4297,16 +4318,16 @@
         <v>217</v>
       </c>
       <c r="D42">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E42" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F42" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="G42" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H42" t="s">
         <v>755</v>
@@ -4318,10 +4339,10 @@
         <v>20</v>
       </c>
       <c r="K42" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="L42" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="M42" t="s">
         <v>23</v>
@@ -4338,16 +4359,16 @@
         <v>217</v>
       </c>
       <c r="D43">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E43" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F43" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G43" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H43" t="s">
         <v>755</v>
@@ -4359,10 +4380,10 @@
         <v>20</v>
       </c>
       <c r="K43" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="L43" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="M43" t="s">
         <v>23</v>
@@ -4379,16 +4400,16 @@
         <v>217</v>
       </c>
       <c r="D44">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E44" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F44" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G44" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H44" t="s">
         <v>755</v>
@@ -4400,10 +4421,10 @@
         <v>20</v>
       </c>
       <c r="K44" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="L44" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="M44" t="s">
         <v>23</v>
@@ -4420,16 +4441,16 @@
         <v>217</v>
       </c>
       <c r="D45">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E45" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F45" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G45" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H45" t="s">
         <v>755</v>
@@ -4441,10 +4462,10 @@
         <v>20</v>
       </c>
       <c r="K45" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="L45" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="M45" t="s">
         <v>23</v>
@@ -4461,16 +4482,16 @@
         <v>217</v>
       </c>
       <c r="D46">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E46" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F46" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G46" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H46" t="s">
         <v>755</v>
@@ -4482,7 +4503,7 @@
         <v>20</v>
       </c>
       <c r="K46" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="L46" t="s">
         <v>247</v>
@@ -4502,16 +4523,16 @@
         <v>217</v>
       </c>
       <c r="D47">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E47" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F47" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G47" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H47" t="s">
         <v>755</v>
@@ -4523,10 +4544,10 @@
         <v>20</v>
       </c>
       <c r="K47" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="L47" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="M47" t="s">
         <v>23</v>
@@ -4543,19 +4564,19 @@
         <v>217</v>
       </c>
       <c r="D48">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E48" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F48" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G48" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H48" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="I48" t="s">
         <v>64</v>
@@ -4564,10 +4585,10 @@
         <v>20</v>
       </c>
       <c r="K48" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="L48" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="M48" t="s">
         <v>23</v>
@@ -4584,16 +4605,16 @@
         <v>217</v>
       </c>
       <c r="D49">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F49" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="G49" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H49" t="s">
         <v>756</v>
@@ -4605,10 +4626,10 @@
         <v>20</v>
       </c>
       <c r="K49" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="L49" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="M49" t="s">
         <v>23</v>
@@ -4622,19 +4643,19 @@
         <v>168</v>
       </c>
       <c r="C50" t="s">
-        <v>267</v>
+        <v>217</v>
       </c>
       <c r="D50">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E50" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="F50" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="G50" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="H50" t="s">
         <v>756</v>
@@ -4646,10 +4667,10 @@
         <v>20</v>
       </c>
       <c r="K50" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="L50" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="M50" t="s">
         <v>23</v>
@@ -4666,16 +4687,16 @@
         <v>267</v>
       </c>
       <c r="D51">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E51" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="F51" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="G51" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="H51" t="s">
         <v>756</v>
@@ -4687,10 +4708,10 @@
         <v>20</v>
       </c>
       <c r="K51" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="L51" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="M51" t="s">
         <v>23</v>
@@ -4707,16 +4728,16 @@
         <v>267</v>
       </c>
       <c r="D52">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F52" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="G52" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H52" t="s">
         <v>756</v>
@@ -4728,10 +4749,10 @@
         <v>20</v>
       </c>
       <c r="K52" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="L52" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="M52" t="s">
         <v>23</v>
@@ -4745,22 +4766,22 @@
         <v>168</v>
       </c>
       <c r="C53" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="D53">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E53" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F53" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G53" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="H53" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="I53" t="s">
         <v>64</v>
@@ -4769,10 +4790,10 @@
         <v>20</v>
       </c>
       <c r="K53" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="L53" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="M53" t="s">
         <v>23</v>
@@ -4789,16 +4810,16 @@
         <v>283</v>
       </c>
       <c r="D54">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E54" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F54" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="G54" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H54" t="s">
         <v>755</v>
@@ -4810,10 +4831,10 @@
         <v>20</v>
       </c>
       <c r="K54" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="L54" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="M54" t="s">
         <v>23</v>
@@ -4830,16 +4851,16 @@
         <v>283</v>
       </c>
       <c r="D55">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E55" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F55" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G55" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="H55" t="s">
         <v>755</v>
@@ -4851,10 +4872,10 @@
         <v>20</v>
       </c>
       <c r="K55" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="L55" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="M55" t="s">
         <v>23</v>
@@ -4871,19 +4892,19 @@
         <v>283</v>
       </c>
       <c r="D56">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E56" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F56" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="G56" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="H56" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="I56" t="s">
         <v>64</v>
@@ -4892,10 +4913,10 @@
         <v>20</v>
       </c>
       <c r="K56" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="L56" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="M56" t="s">
         <v>23</v>
@@ -4912,16 +4933,16 @@
         <v>283</v>
       </c>
       <c r="D57">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E57" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="F57" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="G57" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H57" t="s">
         <v>756</v>
@@ -4933,10 +4954,10 @@
         <v>20</v>
       </c>
       <c r="K57" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="L57" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="M57" t="s">
         <v>23</v>
@@ -4953,16 +4974,16 @@
         <v>283</v>
       </c>
       <c r="D58">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E58" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F58" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="G58" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="H58" t="s">
         <v>756</v>
@@ -4974,10 +4995,10 @@
         <v>20</v>
       </c>
       <c r="K58" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="L58" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="M58" t="s">
         <v>23</v>
@@ -4994,16 +5015,16 @@
         <v>283</v>
       </c>
       <c r="D59">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="F59" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G59" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H59" t="s">
         <v>756</v>
@@ -5015,10 +5036,10 @@
         <v>20</v>
       </c>
       <c r="K59" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="L59" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="M59" t="s">
         <v>23</v>
@@ -5026,43 +5047,43 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>319</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>320</v>
+        <v>168</v>
       </c>
       <c r="C60" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
       <c r="D60">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E60" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="F60" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="G60" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="H60" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="I60" t="s">
         <v>64</v>
       </c>
       <c r="J60" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="K60" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="L60" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="M60" t="s">
-        <v>327</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
@@ -5076,16 +5097,16 @@
         <v>321</v>
       </c>
       <c r="D61">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E61" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="F61" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="G61" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="H61" t="s">
         <v>757</v>
@@ -5097,10 +5118,10 @@
         <v>43</v>
       </c>
       <c r="K61" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="L61" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="M61" t="s">
         <v>327</v>
@@ -5117,16 +5138,16 @@
         <v>321</v>
       </c>
       <c r="D62">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E62" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F62" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="G62" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="H62" t="s">
         <v>757</v>
@@ -5138,10 +5159,10 @@
         <v>43</v>
       </c>
       <c r="K62" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="L62" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="M62" t="s">
         <v>327</v>
@@ -5158,16 +5179,16 @@
         <v>321</v>
       </c>
       <c r="D63">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E63" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F63" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G63" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="H63" t="s">
         <v>757</v>
@@ -5179,10 +5200,10 @@
         <v>43</v>
       </c>
       <c r="K63" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="L63" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="M63" t="s">
         <v>327</v>
@@ -5199,16 +5220,16 @@
         <v>321</v>
       </c>
       <c r="D64">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E64" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="F64" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G64" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="H64" t="s">
         <v>757</v>
@@ -5220,10 +5241,10 @@
         <v>43</v>
       </c>
       <c r="K64" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="L64" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="M64" t="s">
         <v>327</v>
@@ -5240,16 +5261,16 @@
         <v>321</v>
       </c>
       <c r="D65">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E65" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="F65" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="G65" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="H65" t="s">
         <v>757</v>
@@ -5261,10 +5282,10 @@
         <v>43</v>
       </c>
       <c r="K65" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="L65" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="M65" t="s">
         <v>327</v>
@@ -5281,16 +5302,16 @@
         <v>321</v>
       </c>
       <c r="D66">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E66" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="F66" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="G66" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="H66" t="s">
         <v>757</v>
@@ -5302,10 +5323,10 @@
         <v>43</v>
       </c>
       <c r="K66" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="L66" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="M66" t="s">
         <v>327</v>
@@ -5322,16 +5343,16 @@
         <v>321</v>
       </c>
       <c r="D67">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E67" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="F67" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="G67" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="H67" t="s">
         <v>757</v>
@@ -5343,10 +5364,10 @@
         <v>43</v>
       </c>
       <c r="K67" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="L67" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="M67" t="s">
         <v>327</v>
@@ -5363,16 +5384,16 @@
         <v>321</v>
       </c>
       <c r="D68">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E68" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="F68" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="G68" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="H68" t="s">
         <v>757</v>
@@ -5384,10 +5405,10 @@
         <v>43</v>
       </c>
       <c r="K68" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L68" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="M68" t="s">
         <v>327</v>
@@ -5401,19 +5422,19 @@
         <v>320</v>
       </c>
       <c r="C69" t="s">
-        <v>368</v>
+        <v>321</v>
       </c>
       <c r="D69">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E69" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F69" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="G69" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H69" t="s">
         <v>757</v>
@@ -5425,10 +5446,10 @@
         <v>43</v>
       </c>
       <c r="K69" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="L69" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="M69" t="s">
         <v>327</v>
@@ -5445,16 +5466,16 @@
         <v>368</v>
       </c>
       <c r="D70">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E70" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F70" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="G70" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="H70" t="s">
         <v>757</v>
@@ -5466,10 +5487,10 @@
         <v>43</v>
       </c>
       <c r="K70" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="L70" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="M70" t="s">
         <v>327</v>
@@ -5486,16 +5507,16 @@
         <v>368</v>
       </c>
       <c r="D71">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E71" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="F71" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="G71" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="H71" t="s">
         <v>757</v>
@@ -5507,10 +5528,10 @@
         <v>43</v>
       </c>
       <c r="K71" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="L71" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="M71" t="s">
         <v>327</v>
@@ -5527,16 +5548,16 @@
         <v>368</v>
       </c>
       <c r="D72">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E72" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="F72" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="G72" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="H72" t="s">
         <v>757</v>
@@ -5548,10 +5569,10 @@
         <v>43</v>
       </c>
       <c r="K72" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="L72" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="M72" t="s">
         <v>327</v>
@@ -5568,16 +5589,16 @@
         <v>368</v>
       </c>
       <c r="D73">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E73" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="F73" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="G73" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="H73" t="s">
         <v>757</v>
@@ -5589,10 +5610,10 @@
         <v>43</v>
       </c>
       <c r="K73" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="L73" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="M73" t="s">
         <v>327</v>
@@ -5609,16 +5630,16 @@
         <v>368</v>
       </c>
       <c r="D74">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E74" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F74" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="G74" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H74" t="s">
         <v>757</v>
@@ -5630,10 +5651,10 @@
         <v>43</v>
       </c>
       <c r="K74" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="L74" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="M74" t="s">
         <v>327</v>
@@ -5644,37 +5665,37 @@
         <v>319</v>
       </c>
       <c r="B75" t="s">
-        <v>399</v>
+        <v>320</v>
       </c>
       <c r="C75" t="s">
-        <v>399</v>
+        <v>368</v>
       </c>
       <c r="D75">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E75" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="F75" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G75" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="H75" t="s">
-        <v>751</v>
+        <v>757</v>
       </c>
       <c r="I75" t="s">
         <v>64</v>
       </c>
       <c r="J75" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="K75" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="L75" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="M75" t="s">
         <v>327</v>
@@ -5691,16 +5712,16 @@
         <v>399</v>
       </c>
       <c r="D76">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E76" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F76" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G76" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="H76" t="s">
         <v>751</v>
@@ -5712,10 +5733,10 @@
         <v>20</v>
       </c>
       <c r="K76" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="L76" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="M76" t="s">
         <v>327</v>
@@ -5732,31 +5753,31 @@
         <v>399</v>
       </c>
       <c r="D77">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E77" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F77" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="G77" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="H77" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="I77" t="s">
         <v>64</v>
       </c>
       <c r="J77" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="K77" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="L77" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="M77" t="s">
         <v>327</v>
@@ -5773,16 +5794,16 @@
         <v>399</v>
       </c>
       <c r="D78">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E78" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F78" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G78" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="H78" t="s">
         <v>757</v>
@@ -5794,10 +5815,10 @@
         <v>43</v>
       </c>
       <c r="K78" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="L78" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="M78" t="s">
         <v>327</v>
@@ -5814,16 +5835,16 @@
         <v>399</v>
       </c>
       <c r="D79">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E79" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F79" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="G79" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="H79" t="s">
         <v>757</v>
@@ -5835,10 +5856,10 @@
         <v>43</v>
       </c>
       <c r="K79" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="L79" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="M79" t="s">
         <v>327</v>
@@ -5849,37 +5870,37 @@
         <v>319</v>
       </c>
       <c r="B80" t="s">
-        <v>425</v>
+        <v>399</v>
       </c>
       <c r="C80" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
       <c r="D80">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E80" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="F80" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="G80" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="H80" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="I80" t="s">
         <v>64</v>
       </c>
       <c r="J80" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="K80" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="L80" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="M80" t="s">
         <v>327</v>
@@ -5896,16 +5917,16 @@
         <v>426</v>
       </c>
       <c r="D81">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E81" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F81" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G81" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="H81" t="s">
         <v>758</v>
@@ -5917,10 +5938,10 @@
         <v>20</v>
       </c>
       <c r="K81" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="L81" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="M81" t="s">
         <v>327</v>
@@ -5937,19 +5958,19 @@
         <v>426</v>
       </c>
       <c r="D82">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E82" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="F82" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G82" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="H82" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="I82" t="s">
         <v>64</v>
@@ -5958,10 +5979,10 @@
         <v>20</v>
       </c>
       <c r="K82" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="L82" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="M82" t="s">
         <v>327</v>
@@ -5978,16 +5999,16 @@
         <v>426</v>
       </c>
       <c r="D83">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E83" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="F83" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="G83" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="H83" t="s">
         <v>749</v>
@@ -5999,10 +6020,10 @@
         <v>20</v>
       </c>
       <c r="K83" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="L83" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="M83" t="s">
         <v>327</v>
@@ -6019,16 +6040,16 @@
         <v>426</v>
       </c>
       <c r="D84">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E84" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="F84" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="G84" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="H84" t="s">
         <v>749</v>
@@ -6040,10 +6061,10 @@
         <v>20</v>
       </c>
       <c r="K84" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="L84" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="M84" t="s">
         <v>327</v>
@@ -6060,16 +6081,16 @@
         <v>426</v>
       </c>
       <c r="D85">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E85" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="F85" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="G85" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="H85" t="s">
         <v>749</v>
@@ -6081,10 +6102,10 @@
         <v>20</v>
       </c>
       <c r="K85" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="L85" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="M85" t="s">
         <v>327</v>
@@ -6098,22 +6119,22 @@
         <v>425</v>
       </c>
       <c r="C86" t="s">
-        <v>457</v>
+        <v>426</v>
       </c>
       <c r="D86">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E86" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="F86" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="G86" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="H86" t="s">
-        <v>758</v>
+        <v>749</v>
       </c>
       <c r="I86" t="s">
         <v>64</v>
@@ -6122,10 +6143,10 @@
         <v>20</v>
       </c>
       <c r="K86" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="L86" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="M86" t="s">
         <v>327</v>
@@ -6142,16 +6163,16 @@
         <v>457</v>
       </c>
       <c r="D87">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E87" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="F87" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="G87" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="H87" t="s">
         <v>758</v>
@@ -6163,10 +6184,10 @@
         <v>20</v>
       </c>
       <c r="K87" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="L87" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="M87" t="s">
         <v>327</v>
@@ -6183,16 +6204,16 @@
         <v>457</v>
       </c>
       <c r="D88">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E88" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="F88" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="G88" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="H88" t="s">
         <v>758</v>
@@ -6204,10 +6225,10 @@
         <v>20</v>
       </c>
       <c r="K88" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="L88" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="M88" t="s">
         <v>327</v>
@@ -6224,19 +6245,19 @@
         <v>457</v>
       </c>
       <c r="D89">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E89" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F89" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="G89" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="H89" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="I89" t="s">
         <v>64</v>
@@ -6245,10 +6266,10 @@
         <v>20</v>
       </c>
       <c r="K89" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="L89" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="M89" t="s">
         <v>327</v>
@@ -6265,16 +6286,16 @@
         <v>457</v>
       </c>
       <c r="D90">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E90" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="F90" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="G90" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="H90" t="s">
         <v>749</v>
@@ -6286,10 +6307,10 @@
         <v>20</v>
       </c>
       <c r="K90" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="L90" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="M90" t="s">
         <v>327</v>
@@ -6306,16 +6327,16 @@
         <v>457</v>
       </c>
       <c r="D91">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E91" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="F91" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="G91" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="H91" t="s">
         <v>749</v>
@@ -6327,10 +6348,10 @@
         <v>20</v>
       </c>
       <c r="K91" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="L91" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="M91" t="s">
         <v>327</v>
@@ -6347,16 +6368,16 @@
         <v>457</v>
       </c>
       <c r="D92">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E92" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="F92" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="G92" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H92" t="s">
         <v>749</v>
@@ -6368,10 +6389,10 @@
         <v>20</v>
       </c>
       <c r="K92" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="L92" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="M92" t="s">
         <v>327</v>
@@ -6385,22 +6406,22 @@
         <v>425</v>
       </c>
       <c r="C93" t="s">
-        <v>493</v>
+        <v>457</v>
       </c>
       <c r="D93">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E93" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F93" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="G93" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="H93" t="s">
-        <v>758</v>
+        <v>749</v>
       </c>
       <c r="I93" t="s">
         <v>64</v>
@@ -6409,10 +6430,10 @@
         <v>20</v>
       </c>
       <c r="K93" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="L93" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="M93" t="s">
         <v>327</v>
@@ -6429,16 +6450,16 @@
         <v>493</v>
       </c>
       <c r="D94">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E94" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="F94" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="G94" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="H94" t="s">
         <v>758</v>
@@ -6450,10 +6471,10 @@
         <v>20</v>
       </c>
       <c r="K94" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="L94" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="M94" t="s">
         <v>327</v>
@@ -6467,37 +6488,37 @@
         <v>425</v>
       </c>
       <c r="C95" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="D95">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E95" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="F95" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="G95" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="H95" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I95" t="s">
-        <v>161</v>
+        <v>64</v>
       </c>
       <c r="J95" t="s">
         <v>20</v>
       </c>
       <c r="K95" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="L95" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="M95" t="s">
-        <v>23</v>
+        <v>327</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
@@ -6511,16 +6532,16 @@
         <v>504</v>
       </c>
       <c r="D96">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E96" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F96" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="G96" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="H96" t="s">
         <v>759</v>
@@ -6532,10 +6553,10 @@
         <v>20</v>
       </c>
       <c r="K96" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="L96" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="M96" t="s">
         <v>23</v>
@@ -6552,16 +6573,16 @@
         <v>504</v>
       </c>
       <c r="D97">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E97" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="F97" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="G97" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="H97" t="s">
         <v>759</v>
@@ -6573,10 +6594,10 @@
         <v>20</v>
       </c>
       <c r="K97" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="L97" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="M97" t="s">
         <v>23</v>
@@ -6593,31 +6614,31 @@
         <v>504</v>
       </c>
       <c r="D98">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E98" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="F98" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="G98" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="H98" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="I98" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="J98" t="s">
         <v>20</v>
       </c>
       <c r="K98" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="L98" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="M98" t="s">
         <v>23</v>
@@ -6634,16 +6655,16 @@
         <v>504</v>
       </c>
       <c r="D99">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E99" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="F99" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="G99" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="H99" t="s">
         <v>758</v>
@@ -6655,10 +6676,10 @@
         <v>20</v>
       </c>
       <c r="K99" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="L99" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="M99" t="s">
         <v>23</v>
@@ -6675,19 +6696,19 @@
         <v>504</v>
       </c>
       <c r="D100">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E100" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="F100" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="G100" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="H100" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="I100" t="s">
         <v>64</v>
@@ -6696,10 +6717,10 @@
         <v>20</v>
       </c>
       <c r="K100" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="L100" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="M100" t="s">
         <v>23</v>
@@ -6716,16 +6737,16 @@
         <v>504</v>
       </c>
       <c r="D101">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E101" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="F101" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="G101" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="H101" t="s">
         <v>749</v>
@@ -6737,10 +6758,10 @@
         <v>20</v>
       </c>
       <c r="K101" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="L101" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="M101" t="s">
         <v>23</v>
@@ -6751,40 +6772,40 @@
         <v>319</v>
       </c>
       <c r="B102" t="s">
-        <v>540</v>
+        <v>425</v>
       </c>
       <c r="C102" t="s">
-        <v>540</v>
+        <v>504</v>
       </c>
       <c r="D102">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E102" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="F102" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="G102" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="H102" t="s">
-        <v>540</v>
+        <v>749</v>
       </c>
       <c r="I102" t="s">
-        <v>161</v>
+        <v>64</v>
       </c>
       <c r="J102" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="K102" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="L102" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="M102" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.35">
@@ -6798,16 +6819,16 @@
         <v>540</v>
       </c>
       <c r="D103">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E103" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="F103" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="G103" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="H103" t="s">
         <v>540</v>
@@ -6819,10 +6840,10 @@
         <v>43</v>
       </c>
       <c r="K103" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="L103" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="M103" t="s">
         <v>46</v>
@@ -6839,16 +6860,16 @@
         <v>540</v>
       </c>
       <c r="D104">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E104" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="F104" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="G104" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="H104" t="s">
         <v>540</v>
@@ -6860,10 +6881,10 @@
         <v>43</v>
       </c>
       <c r="K104" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="L104" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="M104" t="s">
         <v>46</v>
@@ -6880,16 +6901,16 @@
         <v>540</v>
       </c>
       <c r="D105">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E105" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="F105" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="G105" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="H105" t="s">
         <v>540</v>
@@ -6901,10 +6922,10 @@
         <v>43</v>
       </c>
       <c r="K105" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="L105" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="M105" t="s">
         <v>46</v>
@@ -6921,16 +6942,16 @@
         <v>540</v>
       </c>
       <c r="D106">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E106" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="F106" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="G106" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="H106" t="s">
         <v>540</v>
@@ -6942,10 +6963,10 @@
         <v>43</v>
       </c>
       <c r="K106" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="L106" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="M106" t="s">
         <v>46</v>
@@ -6962,16 +6983,16 @@
         <v>540</v>
       </c>
       <c r="D107">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E107" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="F107" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="G107" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="H107" t="s">
         <v>540</v>
@@ -6983,10 +7004,10 @@
         <v>43</v>
       </c>
       <c r="K107" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="L107" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="M107" t="s">
         <v>46</v>
@@ -7003,16 +7024,16 @@
         <v>540</v>
       </c>
       <c r="D108">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E108" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="F108" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="G108" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="H108" t="s">
         <v>540</v>
@@ -7024,10 +7045,10 @@
         <v>43</v>
       </c>
       <c r="K108" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="L108" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="M108" t="s">
         <v>46</v>
@@ -7044,16 +7065,16 @@
         <v>540</v>
       </c>
       <c r="D109">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E109" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="F109" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="G109" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="H109" t="s">
         <v>540</v>
@@ -7065,10 +7086,10 @@
         <v>43</v>
       </c>
       <c r="K109" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="L109" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M109" t="s">
         <v>46</v>
@@ -7085,16 +7106,16 @@
         <v>540</v>
       </c>
       <c r="D110">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E110" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="F110" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="G110" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="H110" t="s">
         <v>540</v>
@@ -7106,10 +7127,10 @@
         <v>43</v>
       </c>
       <c r="K110" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="L110" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="M110" t="s">
         <v>46</v>
@@ -7126,16 +7147,16 @@
         <v>540</v>
       </c>
       <c r="D111">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E111" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="F111" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="G111" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="H111" t="s">
         <v>540</v>
@@ -7147,10 +7168,10 @@
         <v>43</v>
       </c>
       <c r="K111" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="L111" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="M111" t="s">
         <v>46</v>
@@ -7167,16 +7188,16 @@
         <v>540</v>
       </c>
       <c r="D112">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E112" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="F112" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="G112" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="H112" t="s">
         <v>540</v>
@@ -7188,10 +7209,10 @@
         <v>43</v>
       </c>
       <c r="K112" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="L112" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="M112" t="s">
         <v>46</v>
@@ -7208,28 +7229,31 @@
         <v>540</v>
       </c>
       <c r="D113">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E113" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="F113" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="G113" t="s">
-        <v>598</v>
+        <v>593</v>
+      </c>
+      <c r="H113" t="s">
+        <v>540</v>
       </c>
       <c r="I113" t="s">
-        <v>599</v>
+        <v>161</v>
       </c>
       <c r="J113" t="s">
         <v>43</v>
       </c>
       <c r="K113" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="L113" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="M113" t="s">
         <v>46</v>
@@ -7237,40 +7261,37 @@
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>602</v>
+        <v>319</v>
       </c>
       <c r="B114" t="s">
-        <v>603</v>
+        <v>540</v>
       </c>
       <c r="C114" t="s">
-        <v>604</v>
+        <v>540</v>
       </c>
       <c r="D114">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E114" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="F114" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="G114" t="s">
-        <v>607</v>
-      </c>
-      <c r="H114" t="s">
-        <v>760</v>
+        <v>598</v>
       </c>
       <c r="I114" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="J114" t="s">
         <v>43</v>
       </c>
       <c r="K114" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="L114" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
       <c r="M114" t="s">
         <v>46</v>
@@ -7287,34 +7308,34 @@
         <v>604</v>
       </c>
       <c r="D115">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E115" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="F115" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="G115" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H115" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I115" t="s">
-        <v>64</v>
+        <v>608</v>
       </c>
       <c r="J115" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="K115" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="L115" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="M115" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.35">
@@ -7328,16 +7349,16 @@
         <v>604</v>
       </c>
       <c r="D116">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E116" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="F116" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="G116" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="H116" t="s">
         <v>761</v>
@@ -7349,10 +7370,10 @@
         <v>20</v>
       </c>
       <c r="K116" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="L116" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="M116" t="s">
         <v>23</v>
@@ -7369,16 +7390,16 @@
         <v>604</v>
       </c>
       <c r="D117">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E117" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="F117" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="G117" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="H117" t="s">
         <v>761</v>
@@ -7390,10 +7411,10 @@
         <v>20</v>
       </c>
       <c r="K117" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="L117" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="M117" t="s">
         <v>23</v>
@@ -7410,16 +7431,16 @@
         <v>604</v>
       </c>
       <c r="D118">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E118" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="F118" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="G118" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="H118" t="s">
         <v>761</v>
@@ -7428,16 +7449,16 @@
         <v>64</v>
       </c>
       <c r="J118" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="K118" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="L118" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="M118" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.35">
@@ -7451,16 +7472,16 @@
         <v>604</v>
       </c>
       <c r="D119">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E119" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="F119" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="G119" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="H119" t="s">
         <v>761</v>
@@ -7472,10 +7493,10 @@
         <v>43</v>
       </c>
       <c r="K119" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="L119" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="M119" t="s">
         <v>46</v>
@@ -7489,37 +7510,37 @@
         <v>603</v>
       </c>
       <c r="C120" t="s">
-        <v>636</v>
+        <v>604</v>
       </c>
       <c r="D120">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E120" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="F120" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="G120" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="H120" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="I120" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="J120" t="s">
         <v>43</v>
       </c>
       <c r="K120" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="L120" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="M120" t="s">
-        <v>327</v>
+        <v>46</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.35">
@@ -7533,16 +7554,16 @@
         <v>636</v>
       </c>
       <c r="D121">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E121" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="F121" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="G121" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="H121" t="s">
         <v>762</v>
@@ -7554,10 +7575,10 @@
         <v>43</v>
       </c>
       <c r="K121" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="L121" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="M121" t="s">
         <v>327</v>
@@ -7574,16 +7595,16 @@
         <v>636</v>
       </c>
       <c r="D122">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E122" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="F122" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="G122" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="H122" t="s">
         <v>762</v>
@@ -7595,13 +7616,13 @@
         <v>43</v>
       </c>
       <c r="K122" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="L122" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="M122" t="s">
-        <v>46</v>
+        <v>327</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.35">
@@ -7615,16 +7636,16 @@
         <v>636</v>
       </c>
       <c r="D123">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E123" t="s">
-        <v>15</v>
+        <v>647</v>
       </c>
       <c r="F123" t="s">
-        <v>40</v>
+        <v>648</v>
       </c>
       <c r="G123" t="s">
-        <v>41</v>
+        <v>649</v>
       </c>
       <c r="H123" t="s">
         <v>762</v>
@@ -7636,10 +7657,10 @@
         <v>43</v>
       </c>
       <c r="K123" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="L123" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="M123" t="s">
         <v>46</v>
@@ -7656,16 +7677,16 @@
         <v>636</v>
       </c>
       <c r="D124">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E124" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F124" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G124" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H124" t="s">
         <v>762</v>
@@ -7677,10 +7698,10 @@
         <v>43</v>
       </c>
       <c r="K124" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="L124" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="M124" t="s">
         <v>46</v>
@@ -7697,16 +7718,16 @@
         <v>636</v>
       </c>
       <c r="D125">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E125" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F125" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G125" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H125" t="s">
         <v>762</v>
@@ -7718,10 +7739,10 @@
         <v>43</v>
       </c>
       <c r="K125" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="L125" t="s">
-        <v>54</v>
+        <v>655</v>
       </c>
       <c r="M125" t="s">
         <v>46</v>
@@ -7738,16 +7759,16 @@
         <v>636</v>
       </c>
       <c r="D126">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E126" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F126" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G126" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H126" t="s">
         <v>762</v>
@@ -7759,10 +7780,10 @@
         <v>43</v>
       </c>
       <c r="K126" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="L126" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M126" t="s">
         <v>46</v>
@@ -7779,16 +7800,16 @@
         <v>636</v>
       </c>
       <c r="D127">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E127" t="s">
-        <v>658</v>
+        <v>34</v>
       </c>
       <c r="F127" t="s">
-        <v>659</v>
+        <v>55</v>
       </c>
       <c r="G127" t="s">
-        <v>660</v>
+        <v>56</v>
       </c>
       <c r="H127" t="s">
         <v>762</v>
@@ -7800,10 +7821,10 @@
         <v>43</v>
       </c>
       <c r="K127" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="L127" t="s">
-        <v>662</v>
+        <v>58</v>
       </c>
       <c r="M127" t="s">
         <v>46</v>
@@ -7820,16 +7841,16 @@
         <v>636</v>
       </c>
       <c r="D128">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E128" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="F128" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="G128" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="H128" t="s">
         <v>762</v>
@@ -7841,10 +7862,10 @@
         <v>43</v>
       </c>
       <c r="K128" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="L128" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="M128" t="s">
         <v>46</v>
@@ -7861,16 +7882,16 @@
         <v>636</v>
       </c>
       <c r="D129">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E129" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="F129" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="G129" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="H129" t="s">
         <v>762</v>
@@ -7882,10 +7903,10 @@
         <v>43</v>
       </c>
       <c r="K129" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="L129" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="M129" t="s">
         <v>46</v>
@@ -7902,16 +7923,16 @@
         <v>636</v>
       </c>
       <c r="D130">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E130" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="F130" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="G130" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="H130" t="s">
         <v>762</v>
@@ -7923,13 +7944,13 @@
         <v>43</v>
       </c>
       <c r="K130" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="L130" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="M130" t="s">
-        <v>327</v>
+        <v>46</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.35">
@@ -7940,37 +7961,37 @@
         <v>603</v>
       </c>
       <c r="C131" t="s">
-        <v>678</v>
+        <v>636</v>
       </c>
       <c r="D131">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E131" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="F131" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="G131" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="H131" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="I131" t="s">
-        <v>161</v>
+        <v>42</v>
       </c>
       <c r="J131" t="s">
         <v>43</v>
       </c>
       <c r="K131" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="L131" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="M131" t="s">
-        <v>46</v>
+        <v>327</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.35">
@@ -7984,16 +8005,16 @@
         <v>678</v>
       </c>
       <c r="D132">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E132" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="F132" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="G132" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="H132" t="s">
         <v>763</v>
@@ -8005,10 +8026,10 @@
         <v>43</v>
       </c>
       <c r="K132" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="L132" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="M132" t="s">
         <v>46</v>
@@ -8025,16 +8046,16 @@
         <v>678</v>
       </c>
       <c r="D133">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E133" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="F133" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="G133" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="H133" t="s">
         <v>763</v>
@@ -8046,10 +8067,10 @@
         <v>43</v>
       </c>
       <c r="K133" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="L133" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="M133" t="s">
         <v>46</v>
@@ -8066,16 +8087,16 @@
         <v>678</v>
       </c>
       <c r="D134">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E134" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="F134" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="G134" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="H134" t="s">
         <v>763</v>
@@ -8087,10 +8108,10 @@
         <v>43</v>
       </c>
       <c r="K134" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="L134" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="M134" t="s">
         <v>46</v>
@@ -8107,16 +8128,16 @@
         <v>678</v>
       </c>
       <c r="D135">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E135" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="F135" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="G135" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="H135" t="s">
         <v>763</v>
@@ -8128,10 +8149,10 @@
         <v>43</v>
       </c>
       <c r="K135" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="L135" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="M135" t="s">
         <v>46</v>
@@ -8142,40 +8163,40 @@
         <v>602</v>
       </c>
       <c r="B136" t="s">
-        <v>704</v>
+        <v>603</v>
       </c>
       <c r="C136" t="s">
-        <v>705</v>
+        <v>678</v>
       </c>
       <c r="D136">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E136" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="F136" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="G136" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="H136" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="I136" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="J136" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="K136" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="L136" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="M136" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.35">
@@ -8189,16 +8210,16 @@
         <v>705</v>
       </c>
       <c r="D137">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E137" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="F137" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="G137" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="H137" t="s">
         <v>764</v>
@@ -8210,10 +8231,10 @@
         <v>20</v>
       </c>
       <c r="K137" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="L137" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="M137" t="s">
         <v>23</v>
@@ -8230,16 +8251,16 @@
         <v>705</v>
       </c>
       <c r="D138">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E138" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="F138" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="G138" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="H138" t="s">
         <v>764</v>
@@ -8251,10 +8272,10 @@
         <v>20</v>
       </c>
       <c r="K138" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="L138" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="M138" t="s">
         <v>23</v>
@@ -8271,16 +8292,16 @@
         <v>705</v>
       </c>
       <c r="D139">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E139" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="F139" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="G139" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="H139" t="s">
         <v>764</v>
@@ -8292,10 +8313,10 @@
         <v>20</v>
       </c>
       <c r="K139" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="L139" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="M139" t="s">
         <v>23</v>
@@ -8309,34 +8330,34 @@
         <v>704</v>
       </c>
       <c r="C140" t="s">
-        <v>726</v>
+        <v>705</v>
       </c>
       <c r="D140">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E140" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="F140" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="G140" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="H140" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="I140" t="s">
-        <v>730</v>
+        <v>64</v>
       </c>
       <c r="J140" t="s">
         <v>20</v>
       </c>
       <c r="K140" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="L140" t="s">
-        <v>732</v>
+        <v>725</v>
       </c>
       <c r="M140" t="s">
         <v>23</v>
@@ -8353,16 +8374,16 @@
         <v>726</v>
       </c>
       <c r="D141">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E141" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="F141" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="G141" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="H141" t="s">
         <v>765</v>
@@ -8374,10 +8395,10 @@
         <v>20</v>
       </c>
       <c r="K141" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="L141" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="M141" t="s">
         <v>23</v>
@@ -8394,16 +8415,16 @@
         <v>726</v>
       </c>
       <c r="D142">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E142" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="F142" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="G142" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="H142" t="s">
         <v>765</v>
@@ -8415,10 +8436,10 @@
         <v>20</v>
       </c>
       <c r="K142" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="L142" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="M142" t="s">
         <v>23</v>
@@ -8435,16 +8456,16 @@
         <v>726</v>
       </c>
       <c r="D143">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E143" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="F143" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="G143" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="H143" t="s">
         <v>765</v>
@@ -8456,12 +8477,53 @@
         <v>20</v>
       </c>
       <c r="K143" t="s">
+        <v>741</v>
+      </c>
+      <c r="L143" t="s">
+        <v>742</v>
+      </c>
+      <c r="M143" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>602</v>
+      </c>
+      <c r="B144" t="s">
+        <v>704</v>
+      </c>
+      <c r="C144" t="s">
+        <v>726</v>
+      </c>
+      <c r="D144">
+        <v>142</v>
+      </c>
+      <c r="E144" t="s">
+        <v>743</v>
+      </c>
+      <c r="F144" t="s">
+        <v>744</v>
+      </c>
+      <c r="G144" t="s">
+        <v>745</v>
+      </c>
+      <c r="H144" t="s">
+        <v>765</v>
+      </c>
+      <c r="I144" t="s">
+        <v>730</v>
+      </c>
+      <c r="J144" t="s">
+        <v>20</v>
+      </c>
+      <c r="K144" t="s">
         <v>746</v>
       </c>
-      <c r="L143" t="s">
+      <c r="L144" t="s">
         <v>747</v>
       </c>
-      <c r="M143" t="s">
+      <c r="M144" t="s">
         <v>23</v>
       </c>
     </row>
@@ -8481,6 +8543,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="579d0760968303502ff8eb3a8a5e610f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6855c386bbcb23a4cad2dada315b1779" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -8729,17 +8802,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E88BA6A-AC61-4AC2-A996-5A1D6BDE06E6}">
   <ds:schemaRefs>
@@ -8749,6 +8811,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8432CF-B2BE-4FBE-BA17-BEF2C1145140}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B06C0B83-8F91-4FA8-B18E-5FF0700E1417}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8765,15 +8838,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8432CF-B2BE-4FBE-BA17-BEF2C1145140}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>